<commit_message>
Added portion size to nutrients
</commit_message>
<xml_diff>
--- a/BlackBoxUnitTests.xlsx
+++ b/BlackBoxUnitTests.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MacroMate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF7F70-1F56-45AD-8E3F-90D09DA33B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475512C-C08D-4086-9F95-F24B51777E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nutrients_Constructor" sheetId="1" r:id="rId1"/>
+    <sheet name="Nutrients_Scale" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>Test Case</t>
   </si>
@@ -158,6 +159,15 @@
   </si>
   <si>
     <t>all negative</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Nutrients</t>
+  </si>
+  <si>
+    <t>Portion</t>
   </si>
 </sst>
 </file>
@@ -207,9 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -556,24 +569,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.09765625" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,33 +595,35 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
       <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -618,24 +632,27 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2">
+        <v>100</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -644,24 +661,27 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4">
-        <v>100</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="5">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -670,24 +690,27 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="2">
+        <v>100</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -696,24 +719,27 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="2">
+        <v>100</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -722,24 +748,27 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -748,24 +777,27 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="4">
-        <v>100</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="5">
+        <v>100</v>
+      </c>
+      <c r="F8" s="5">
+        <v>100</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -774,24 +806,27 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>100</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+      <c r="E9" s="5">
+        <v>100</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>100</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -800,24 +835,27 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4">
-        <v>100</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>100</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="D10" s="2">
+        <v>100</v>
+      </c>
+      <c r="E10" s="5">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -826,24 +864,27 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>100</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <v>100</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>100</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -852,24 +893,27 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>100</v>
-      </c>
-      <c r="G12" s="4">
-        <v>100</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="D12" s="2">
+        <v>100</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100</v>
+      </c>
+      <c r="H12" s="5">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -878,24 +922,27 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>100</v>
-      </c>
-      <c r="F13" s="4">
-        <v>100</v>
-      </c>
-      <c r="G13" s="4">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="D13" s="2">
+        <v>100</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>100</v>
+      </c>
+      <c r="G13" s="5">
+        <v>100</v>
+      </c>
+      <c r="H13" s="5">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -904,24 +951,27 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4">
-        <v>100</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>100</v>
-      </c>
-      <c r="G14" s="4">
-        <v>100</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="5">
+        <v>100</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>100</v>
+      </c>
+      <c r="H14" s="5">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -930,24 +980,27 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4">
-        <v>100</v>
-      </c>
-      <c r="E15" s="4">
-        <v>100</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>100</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="D15" s="2">
+        <v>100</v>
+      </c>
+      <c r="E15" s="5">
+        <v>100</v>
+      </c>
+      <c r="F15" s="5">
+        <v>100</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -956,24 +1009,27 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="4">
-        <v>100</v>
-      </c>
-      <c r="E16" s="4">
-        <v>100</v>
-      </c>
-      <c r="F16" s="4">
-        <v>100</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="D16" s="2">
+        <v>100</v>
+      </c>
+      <c r="E16" s="5">
+        <v>100</v>
+      </c>
+      <c r="F16" s="5">
+        <v>100</v>
+      </c>
+      <c r="G16" s="5">
+        <v>100</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -982,24 +1038,27 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="4">
-        <v>100</v>
-      </c>
-      <c r="E17" s="4">
-        <v>100</v>
-      </c>
-      <c r="F17" s="4">
-        <v>100</v>
-      </c>
-      <c r="G17" s="4">
-        <v>100</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="D17" s="2">
+        <v>100</v>
+      </c>
+      <c r="E17" s="5">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="G17" s="5">
+        <v>100</v>
+      </c>
+      <c r="H17" s="5">
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1008,24 +1067,27 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="D18" s="2">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1034,24 +1096,27 @@
       <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="2">
+        <v>100</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1060,24 +1125,27 @@
       <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="D20" s="2">
+        <v>100</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1086,24 +1154,27 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="D21" s="2">
+        <v>100</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1112,24 +1183,27 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E22" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="D22" s="2">
+        <v>100</v>
+      </c>
+      <c r="E22" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F22" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1138,24 +1212,27 @@
       <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="D23" s="2">
+        <v>100</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1164,24 +1241,27 @@
       <c r="C24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="D24" s="2">
+        <v>100</v>
+      </c>
+      <c r="E24" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1190,24 +1270,27 @@
       <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="D25" s="2">
+        <v>100</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -1216,24 +1299,27 @@
       <c r="C26" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G26" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="D26" s="2">
+        <v>100</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H26" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -1242,24 +1328,27 @@
       <c r="C27" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F27" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G27" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="D27" s="2">
+        <v>100</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G27" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H27" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -1268,24 +1357,27 @@
       <c r="C28" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G28" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="D28" s="2">
+        <v>100</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H28" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -1294,24 +1386,27 @@
       <c r="C29" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E29" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F29" s="4">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="D29" s="2">
+        <v>100</v>
+      </c>
+      <c r="E29" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -1320,24 +1415,27 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E30" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F30" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G30" s="4">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="D30" s="2">
+        <v>100</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F30" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G30" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -1346,19 +1444,22 @@
       <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="4">
-        <v>-10</v>
-      </c>
-      <c r="E31" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F31" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G31" s="4">
-        <v>-10</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="D31" s="2">
+        <v>100</v>
+      </c>
+      <c r="E31" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G31" s="5">
+        <v>-10</v>
+      </c>
+      <c r="H31" s="5">
+        <v>-10</v>
+      </c>
+      <c r="I31" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1366,7 +1467,51 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E19:G19 B19 A1:C3 E1:H1 E5:H7 E3:H3 G2:H2" numberStoredAsText="1"/>
+    <ignoredError sqref="F19:H19 B19 A1:C3 G1:I1 F5:I7 F3:I3 H2:I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E185B217-D78D-436F-866D-EB8EFF42E387}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed unnecessary  unit tests and added tests for portion property, some fail
</commit_message>
<xml_diff>
--- a/BlackBoxUnitTests.xlsx
+++ b/BlackBoxUnitTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MacroMate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475512C-C08D-4086-9F95-F24B51777E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2ABB2A-A8CC-47F7-A7B3-0BDBC9B3C356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>Test Case</t>
   </si>
@@ -89,33 +89,6 @@
     <t>just fat</t>
   </si>
   <si>
-    <t>calories + protein</t>
-  </si>
-  <si>
-    <t>calories + carbs</t>
-  </si>
-  <si>
-    <t>calories + fat</t>
-  </si>
-  <si>
-    <t>protein + fat</t>
-  </si>
-  <si>
-    <t>carbs + fat</t>
-  </si>
-  <si>
-    <t>no calories</t>
-  </si>
-  <si>
-    <t>no protein</t>
-  </si>
-  <si>
-    <t>no carbs</t>
-  </si>
-  <si>
-    <t>no fat</t>
-  </si>
-  <si>
     <t>Everything</t>
   </si>
   <si>
@@ -131,33 +104,6 @@
     <t>Negative fat</t>
   </si>
   <si>
-    <t>negative cals + protein</t>
-  </si>
-  <si>
-    <t>negative cals + carbs</t>
-  </si>
-  <si>
-    <t>negative cals + fats</t>
-  </si>
-  <si>
-    <t>negative protein + fats</t>
-  </si>
-  <si>
-    <t>negative carbs + fat</t>
-  </si>
-  <si>
-    <t>no negative calories</t>
-  </si>
-  <si>
-    <t>no negative proteins</t>
-  </si>
-  <si>
-    <t>no negative carbs</t>
-  </si>
-  <si>
-    <t>no negative fats</t>
-  </si>
-  <si>
     <t>all negative</t>
   </si>
   <si>
@@ -168,6 +114,12 @@
   </si>
   <si>
     <t>Portion</t>
+  </si>
+  <si>
+    <t>zero portion size</t>
+  </si>
+  <si>
+    <t>Invalid Input negative portion size</t>
   </si>
 </sst>
 </file>
@@ -569,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -607,7 +559,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -787,10 +739,10 @@
         <v>100</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
@@ -801,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -810,19 +762,19 @@
         <v>100</v>
       </c>
       <c r="E9" s="5">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
       </c>
       <c r="G9" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -830,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -839,19 +791,19 @@
         <v>100</v>
       </c>
       <c r="E10" s="5">
-        <v>100</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -859,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -871,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H11" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -888,7 +840,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -903,13 +855,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -917,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -926,19 +878,19 @@
         <v>100</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F13" s="5">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="G13" s="5">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="H13" s="5">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -946,28 +898,28 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
       </c>
       <c r="G14" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -975,499 +927,104 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2">
-        <v>100</v>
+        <v>-10</v>
       </c>
       <c r="E15" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F15" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5">
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2">
-        <v>100</v>
-      </c>
-      <c r="E16" s="5">
-        <v>100</v>
-      </c>
-      <c r="F16" s="5">
-        <v>100</v>
-      </c>
-      <c r="G16" s="5">
-        <v>100</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="2">
-        <v>100</v>
-      </c>
-      <c r="E17" s="5">
-        <v>100</v>
-      </c>
-      <c r="F17" s="5">
-        <v>100</v>
-      </c>
-      <c r="G17" s="5">
-        <v>100</v>
-      </c>
-      <c r="H17" s="5">
-        <v>100</v>
-      </c>
-      <c r="I17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="2">
-        <v>100</v>
-      </c>
-      <c r="E18" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="2">
-        <v>100</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="2">
-        <v>100</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="2">
-        <v>100</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="2">
-        <v>100</v>
-      </c>
-      <c r="E22" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F22" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="2">
-        <v>100</v>
-      </c>
-      <c r="E23" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="2">
-        <v>100</v>
-      </c>
-      <c r="E24" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="2">
-        <v>100</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="2">
-        <v>100</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H26" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2">
-        <v>100</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G27" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H27" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="2">
-        <v>100</v>
-      </c>
-      <c r="E28" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H28" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="2">
-        <v>100</v>
-      </c>
-      <c r="E29" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F29" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2">
-        <v>100</v>
-      </c>
-      <c r="E30" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F30" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G30" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2">
-        <v>100</v>
-      </c>
-      <c r="E31" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F31" s="5">
-        <v>-10</v>
-      </c>
-      <c r="G31" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H31" s="5">
-        <v>-10</v>
-      </c>
-      <c r="I31" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F19:H19 B19 A1:C3 G1:I1 F5:I7 F3:I3 H2:I2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C3 G1:I1 F5:I7 F3:I3 H2:I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1505,10 +1062,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test: Add unit tests for scale method in Nutrients class
</commit_message>
<xml_diff>
--- a/BlackBoxUnitTests.xlsx
+++ b/BlackBoxUnitTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MacroMate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2ABB2A-A8CC-47F7-A7B3-0BDBC9B3C356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E2D366-9157-480A-BBE0-091B3AE5BB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7248" yWindow="3708" windowWidth="14436" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nutrients_Constructor" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Test Case</t>
   </si>
@@ -120,6 +120,24 @@
   </si>
   <si>
     <t>Invalid Input negative portion size</t>
+  </si>
+  <si>
+    <t>Nutrients(100,45,10,1,0)</t>
+  </si>
+  <si>
+    <t>Nutrients(50, 22.5, 5, 0.5, 0)</t>
+  </si>
+  <si>
+    <t>Smaller portion</t>
+  </si>
+  <si>
+    <t>Bigger portion</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Nutrients(200, 90, 20, 2, 0)</t>
   </si>
 </sst>
 </file>
@@ -523,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1031,16 +1049,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E185B217-D78D-436F-866D-EB8EFF42E387}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1068,6 +1088,43 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>